<commit_message>
Update S&S BOM for TL074AC.
</commit_message>
<xml_diff>
--- a/Modules/S&S/S&S_BOM.xlsx
+++ b/Modules/S&S/S&S_BOM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\S&amp;S\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1A2A7E-CC7A-4016-8813-EC1C734A6ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1260" windowWidth="36435" windowHeight="16815"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S&amp;S" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t>Qty</t>
   </si>
@@ -615,9 +621,6 @@
     <t>https://www.tme.eu/hr/en/details/mc5-10n/tht-film-capacitors/kemet/r82ec2100dq50k/</t>
   </si>
   <si>
-    <t>* Do not use the included washer.</t>
-  </si>
-  <si>
     <t>1x4</t>
   </si>
   <si>
@@ -643,6 +646,45 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005002426090397.html</t>
+  </si>
+  <si>
+    <t>D3, D4, D5</t>
+  </si>
+  <si>
+    <t>BZX55C4V7</t>
+  </si>
+  <si>
+    <t>Zener Diode (4.7V)</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/bzx55c4v7-cdi/tht-zener-diodes/cdil/bzx55c4v7/</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>J112</t>
+  </si>
+  <si>
+    <t>N-JFET Transistor</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/j112/tht-n-channel-transistors/onsemi/</t>
+  </si>
+  <si>
+    <t>Purchase in Etsy Store:</t>
+  </si>
+  <si>
+    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
+  </si>
+  <si>
+    <t>U2</t>
   </si>
   <si>
     <r>
@@ -658,51 +700,40 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>**</t>
+    </r>
+  </si>
+  <si>
+    <t>** Do not use the included washer.</t>
+  </si>
+  <si>
+    <t>TL074AC</t>
+  </si>
+  <si>
+    <t>* U1 has to be the AC version of TL074. Other versions might not work correctly.</t>
+  </si>
+  <si>
+    <r>
+      <t>U1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>*</t>
     </r>
-  </si>
-  <si>
-    <t>D3, D4, D5</t>
-  </si>
-  <si>
-    <t>BZX55C4V7</t>
-  </si>
-  <si>
-    <t>Zener Diode (4.7V)</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/bzx55c4v7-cdi/tht-zener-diodes/cdil/bzx55c4v7/</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>J112</t>
-  </si>
-  <si>
-    <t>N-JFET Transistor</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/j112/tht-n-channel-transistors/onsemi/</t>
-  </si>
-  <si>
-    <t>Purchase in Etsy Store:</t>
-  </si>
-  <si>
-    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -896,6 +927,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1239,7 +1278,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1252,6 +1291,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1304,14 +1344,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1349,7 +1392,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1421,7 +1464,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1594,11 +1637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +1752,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,19 +1760,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1963,7 +2006,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
@@ -1977,19 +2020,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
         <v>55</v>
@@ -2026,10 +2069,10 @@
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,16 +2097,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>69</v>
+      <c r="D23" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="E23" t="s">
         <v>63</v>
@@ -2077,19 +2120,19 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,59 +2140,59 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,30 +2200,33 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
+        <v>93</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
@@ -2188,42 +2234,39 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
       </c>
       <c r="E30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>17</v>
+      <c r="D31" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E31" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2231,124 +2274,127 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>33</v>
+        <v>96</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>34</v>
       </c>
+      <c r="F32" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="4"/>
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>117</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>118</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>119</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D37" s="4"/>
-    </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2</v>
-      </c>
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
         <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2356,92 +2402,115 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>97</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>98</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>99</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>123</v>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>2</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="O49" s="6" t="s">
-        <v>145</v>
+      <c r="C51" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2:F11" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html"/>
-    <hyperlink ref="F12" r:id="rId2"/>
-    <hyperlink ref="F13" r:id="rId3"/>
-    <hyperlink ref="F16" r:id="rId4"/>
-    <hyperlink ref="F15" r:id="rId5"/>
-    <hyperlink ref="F17" r:id="rId6"/>
-    <hyperlink ref="F18" r:id="rId7"/>
-    <hyperlink ref="F20" r:id="rId8"/>
-    <hyperlink ref="F23" r:id="rId9"/>
-    <hyperlink ref="F24" r:id="rId10"/>
-    <hyperlink ref="F25" r:id="rId11"/>
-    <hyperlink ref="F26" r:id="rId12"/>
-    <hyperlink ref="F27" r:id="rId13"/>
-    <hyperlink ref="F41" r:id="rId14"/>
-    <hyperlink ref="F34" r:id="rId15"/>
-    <hyperlink ref="F35" r:id="rId16"/>
-    <hyperlink ref="F36" r:id="rId17"/>
-    <hyperlink ref="F14" r:id="rId18"/>
-    <hyperlink ref="F38" r:id="rId19"/>
-    <hyperlink ref="F39" r:id="rId20"/>
-    <hyperlink ref="F30" r:id="rId21"/>
-    <hyperlink ref="F31" r:id="rId22"/>
-    <hyperlink ref="F40" r:id="rId23"/>
-    <hyperlink ref="C49" r:id="rId24"/>
-    <hyperlink ref="F5" r:id="rId25"/>
-    <hyperlink ref="F19" r:id="rId26"/>
-    <hyperlink ref="F6" r:id="rId27"/>
-    <hyperlink ref="F21" r:id="rId28"/>
-    <hyperlink ref="F22" r:id="rId29"/>
-    <hyperlink ref="O49" r:id="rId30"/>
+    <hyperlink ref="F2:F11" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F25" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F26" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F35" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F36" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F37" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F39" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F40" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F31" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F41" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C51" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F5" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F6" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F21" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F22" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="O51" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F23" r:id="rId31" xr:uid="{0DA5FBDE-A9E6-48C7-A3AB-9C6D18E6934A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update S&S for KiCad 8, update capacitor size and BOM.
</commit_message>
<xml_diff>
--- a/Modules/S&S/S&S_BOM.xlsx
+++ b/Modules/S&S/S&S_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\S&amp;S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03579DA3-AD31-402B-B0F9-056446C37D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89189F1E-17EC-4E81-AFE1-DE296D828727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="152">
   <si>
     <t>Qty</t>
   </si>
@@ -68,9 +68,6 @@
     <t>C10</t>
   </si>
   <si>
-    <t>10uF (Film)</t>
-  </si>
-  <si>
     <t>C11</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
   </si>
   <si>
     <t>Capacitor Film THT</t>
-  </si>
-  <si>
-    <t>C-5mm 11x7.2mm</t>
   </si>
   <si>
     <t>C-5mm 2.5x7.2mm</t>
@@ -700,6 +694,37 @@
     <t>U2</t>
   </si>
   <si>
+    <t>https://www.tme.eu/hr/en/details/mks2-2.2u_50-r/tht-film-capacitors/wima/mks2b042201f00ko00/</t>
+  </si>
+  <si>
+    <t>C-5mm 5x7.2 / 11x7.2 mm</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2uF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / 10uF (Film)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Alpha 9mm Nut</t>
     </r>
@@ -715,20 +740,8 @@
       </rPr>
       <t>**</t>
     </r>
-  </si>
-  <si>
-    <t>TL074AC</t>
-  </si>
-  <si>
-    <t>* U1 has to be the AC version of TL074. Other versions might not work correctly.</t>
-  </si>
-  <si>
-    <r>
-      <t>U1</t>
-    </r>
     <r>
       <rPr>
-        <i/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -739,14 +752,38 @@
     </r>
   </si>
   <si>
-    <t>** Do not use the included washer. Tighten very gently so the PCB doesn't get scratched.</t>
+    <t>** U1 has to be the AC version of TL074. Other versions might not work correctly.</t>
+  </si>
+  <si>
+    <t>*** Do not use the included washer. Tighten very gently so the PCB doesn't get scratched.</t>
+  </si>
+  <si>
+    <t>* A 2.2 uF capacitor is the new preferred size. Older modules were built with 10uF, but the slew time was often too long and didn't allow for more suble slews in lower ranges.</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <r>
+      <t>TL074AC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -938,14 +975,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1650,10 +1679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,7 +1695,7 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1683,11 +1712,11 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1695,199 +1724,199 @@
         <v>330</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1895,19 +1924,19 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1915,19 +1944,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1935,39 +1964,42 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1975,16 +2007,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1992,19 +2024,19 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,19 +2044,19 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,19 +2064,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="E19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2052,19 +2084,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,19 +2104,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2092,19 +2124,19 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2112,19 +2144,19 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,19 +2164,19 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2152,19 +2184,19 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2172,19 +2204,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" t="s">
-        <v>52</v>
-      </c>
       <c r="F26" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2192,19 +2224,19 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
-      </c>
       <c r="F27" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2212,19 +2244,19 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2232,16 +2264,16 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2249,16 +2281,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,19 +2298,19 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2286,19 +2318,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2306,16 +2338,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
         <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2326,16 +2358,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
         <v>109</v>
       </c>
-      <c r="C35" t="s">
+      <c r="F35" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2343,16 +2375,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
         <v>113</v>
       </c>
-      <c r="C36" t="s">
+      <c r="F36" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2360,16 +2392,16 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" t="s">
         <v>117</v>
       </c>
-      <c r="C37" t="s">
+      <c r="F37" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="E37" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2380,16 +2412,16 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" t="s">
+        <v>124</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C39" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,16 +2429,16 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2414,16 +2446,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2431,26 +2463,26 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" t="s">
         <v>97</v>
       </c>
-      <c r="C42" t="s">
+      <c r="F42" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="E42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2458,34 +2490,39 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>2</v>
       </c>
-      <c r="B51" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O51" s="6" t="s">
-        <v>143</v>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2494,7 +2531,7 @@
     <hyperlink ref="F12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="P15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="F18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
@@ -2513,16 +2550,17 @@
     <hyperlink ref="F31" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="F32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="F41" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C51" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C52" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="F5" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="F19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="F6" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F21" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="F22" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="O51" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="O52" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="F23" r:id="rId31" xr:uid="{0DA5FBDE-A9E6-48C7-A3AB-9C6D18E6934A}"/>
+    <hyperlink ref="F15" r:id="rId32" xr:uid="{97709935-7D03-4437-A153-F74893B872B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Swap S&S front and back component formatting so it is in line with other modules.
</commit_message>
<xml_diff>
--- a/Modules/S&S/S&S_BOM.xlsx
+++ b/Modules/S&S/S&S_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\S&amp;S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7316EEE-2F4F-4106-B2E3-34C168FCD45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CA34D2-353C-4EA0-9C86-4D8E0C9311C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,272 +224,6 @@
     <t>SPDT ON-ON</t>
   </si>
   <si>
-    <t>Parts in bold are on the front PCB!</t>
-  </si>
-  <si>
-    <t>Parts in itallic are on the back PCB!</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>J_B1, J_B3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, J_D1, J_D2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, R17, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>U1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, U2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, R19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C3, C4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, C5, C6, C7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">R2, R4, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, C12</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>J_A1, J_A3,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J_C1, J_C2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R10, R11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, R20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R5, R6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>240k</t>
   </si>
   <si>
@@ -521,9 +255,6 @@
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/bc547-cdi/npn-tht-transistors/cdil/tbc547/</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005003256812123.html</t>
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/tl074acn/tht-operational-amplifiers/texas-instruments/</t>
@@ -781,12 +512,233 @@
   <si>
     <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, R17, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R10, R11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, R20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, R19</t>
+    </r>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <r>
+      <t>R2, R4,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R12, R14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, C12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C3, C4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, C5, C6, C7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, U2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J_A1, J_A3,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_C1, J_C2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B1, J_B3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, J_D1, J_D2</t>
+    </r>
+  </si>
+  <si>
+    <t>Parts in itallic are on the front PCB!</t>
+  </si>
+  <si>
+    <t>Parts in bold are on the back PCB!</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003256812123.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -947,14 +899,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -978,6 +922,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1321,9 +1280,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1333,9 +1292,10 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1685,7 +1645,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G1" s="3"/>
     </row>
@@ -1729,14 +1689,14 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>78</v>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1749,14 +1709,14 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>66</v>
+      <c r="D3" t="s">
+        <v>140</v>
       </c>
       <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>78</v>
+      <c r="F3" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1775,8 +1735,8 @@
       <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>78</v>
+      <c r="F4" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1795,8 +1755,8 @@
       <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>129</v>
+      <c r="F5" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1804,19 +1764,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>136</v>
+      <c r="D6" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="E6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>129</v>
+      <c r="F6" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1829,14 +1789,14 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>73</v>
+      <c r="D7" t="s">
+        <v>141</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>78</v>
+      <c r="F7" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1849,14 +1809,14 @@
       <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>68</v>
+      <c r="D8" t="s">
+        <v>142</v>
       </c>
       <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>78</v>
+      <c r="F8" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1869,14 +1829,14 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>74</v>
+      <c r="D9" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>78</v>
+      <c r="F9" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1884,19 +1844,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>78</v>
+      <c r="F10" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1910,13 +1870,13 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>78</v>
+      <c r="F11" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1929,14 +1889,14 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>71</v>
+      <c r="D12" t="s">
+        <v>145</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>79</v>
+      <c r="F12" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1949,14 +1909,14 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>69</v>
+      <c r="D13" t="s">
+        <v>146</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>80</v>
+      <c r="F13" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1969,14 +1929,14 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>120</v>
+      <c r="F14" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1984,22 +1944,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>82</v>
+      <c r="F15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2012,14 +1972,14 @@
       <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>81</v>
+      <c r="F16" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2032,14 +1992,14 @@
       <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>83</v>
+      <c r="F17" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2052,14 +2012,14 @@
       <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>130</v>
+      <c r="D18" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>84</v>
+      <c r="F18" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2067,19 +2027,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>133</v>
+      <c r="D19" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>134</v>
+        <v>119</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2098,8 +2058,8 @@
       <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>85</v>
+      <c r="F20" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,19 +2067,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>139</v>
+        <v>125</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,14 +2092,14 @@
       <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>67</v>
+      <c r="D22" t="s">
+        <v>147</v>
       </c>
       <c r="E22" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>86</v>
+      <c r="F22" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,19 +2107,19 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>150</v>
+      <c r="D23" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>87</v>
+      <c r="F23" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2173,13 +2133,13 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>87</v>
+      <c r="F24" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2190,16 +2150,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>88</v>
+        <v>113</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2212,14 +2172,14 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E26" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>89</v>
+      <c r="F26" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2232,14 +2192,14 @@
       <c r="C27" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E27" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>90</v>
+      <c r="F27" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,19 +2207,19 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E28" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>92</v>
+      <c r="F28" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2267,19 +2227,19 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>152</v>
+      <c r="F29" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2287,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -2298,8 +2258,8 @@
       <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>152</v>
+      <c r="F30" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,19 +2267,19 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>65</v>
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>149</v>
       </c>
       <c r="E31" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>127</v>
+      <c r="F31" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2327,19 +2287,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>127</v>
+      <c r="F32" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,12 +2307,12 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E33" t="s">
@@ -2367,16 +2327,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>110</v>
+        <v>96</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2384,16 +2344,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>114</v>
+        <v>100</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,16 +2361,16 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
-        <v>117</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2421,16 +2381,16 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>101</v>
+        <v>111</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2438,16 +2398,16 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>103</v>
+        <v>111</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,16 +2415,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2472,49 +2432,49 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>64</v>
+      <c r="B44" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>63</v>
+      <c r="B45" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>149</v>
+      <c r="B47" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
-        <v>147</v>
+      <c r="B48" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
-        <v>148</v>
+      <c r="B49" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -2522,16 +2482,16 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="O52" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="O52" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2564,11 +2524,11 @@
     <hyperlink ref="F19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="F6" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F21" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="F22" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="O52" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F23" r:id="rId31" xr:uid="{0DA5FBDE-A9E6-48C7-A3AB-9C6D18E6934A}"/>
-    <hyperlink ref="F15" r:id="rId32" xr:uid="{97709935-7D03-4437-A153-F74893B872B7}"/>
-    <hyperlink ref="F29:F30" r:id="rId33" display="https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/" xr:uid="{6D1EC43E-9D04-417C-B22C-F34EBB95F4FB}"/>
+    <hyperlink ref="O52" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F23" r:id="rId30" xr:uid="{0DA5FBDE-A9E6-48C7-A3AB-9C6D18E6934A}"/>
+    <hyperlink ref="F15" r:id="rId31" xr:uid="{97709935-7D03-4437-A153-F74893B872B7}"/>
+    <hyperlink ref="F29:F30" r:id="rId32" display="https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/" xr:uid="{6D1EC43E-9D04-417C-B22C-F34EBB95F4FB}"/>
+    <hyperlink ref="F22" r:id="rId33" xr:uid="{B3BEA3C8-45AF-4461-AEBA-B3CF3A651F54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>

</xml_diff>